<commit_message>
All plots are now implemented
</commit_message>
<xml_diff>
--- a/raw_test_2.xlsx
+++ b/raw_test_2.xlsx
@@ -5,27 +5,33 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmdehaan/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bmdehaan/Documents/Programeren/R/digitoets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E37F122-A627-E040-845F-721F273FC550}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8033866D-A0AD-C24B-AC87-836193995F08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -117,12 +123,6 @@
     <t>Wat vond je van deze vragenlijst?</t>
   </si>
   <si>
-    <t>anonymous</t>
-  </si>
-  <si>
-    <t>Nederlands</t>
-  </si>
-  <si>
     <t>BML-Research</t>
   </si>
   <si>
@@ -132,49 +132,46 @@
     <t>Ja</t>
   </si>
   <si>
-    <t>Je kunt op backspace drukken (je hoeft niet te gummen/krassen) en je hoeft na afloop niet te stuntelen met een camera</t>
-  </si>
-  <si>
-    <t>Soms kun je dingen makkelijker tekenen dan onder woorden brengen.</t>
-  </si>
-  <si>
     <t>Deels oneens</t>
   </si>
   <si>
     <t>Deels eens</t>
   </si>
   <si>
-    <t>Een handleiding die vooraf beschikbaar is op Blackboard;Een oefententamen op Blackboard;Een instructievideo op Blackboard of Kaltura;</t>
-  </si>
-  <si>
     <t>Helemaal eens</t>
   </si>
   <si>
-    <t>Er waren 2 tentamens tegelijk gepland, de docent van 1 van de 2 tentamens heeft toen voor mij (en nog een aantal anderen) een aparte gelegenheid gecreeerd.</t>
-  </si>
-  <si>
-    <t>Ik doe de opleiding research en de minor bioinformatica en ik heb soms het idee dat de research ons vergeet in de planningen, zo worden bijvoorbeeld tentamens dubbel gepland en krijgen wij lang niet alle mails binnen.</t>
-  </si>
-  <si>
-    <t>English (United States)‎</t>
-  </si>
-  <si>
     <t>Leerjaar 1</t>
   </si>
   <si>
-    <t>yghjkm</t>
-  </si>
-  <si>
-    <t>ghbjnkm</t>
-  </si>
-  <si>
     <t>Neutraal</t>
   </si>
   <si>
-    <t>Een instructievideo op Blackboard of Kaltura;</t>
-  </si>
-  <si>
     <t>Nee</t>
+  </si>
+  <si>
+    <t>Leerjaar 2</t>
+  </si>
+  <si>
+    <t>Leerjaar 4</t>
+  </si>
+  <si>
+    <t>Helemaal oneens</t>
+  </si>
+  <si>
+    <t>BML-Diagnostiek</t>
+  </si>
+  <si>
+    <t>Chemie</t>
+  </si>
+  <si>
+    <t>Chemische Technologie</t>
+  </si>
+  <si>
+    <t>Bioinformatica</t>
+  </si>
+  <si>
+    <t>Master Datascience</t>
   </si>
 </sst>
 </file>
@@ -184,7 +181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,16 +189,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor rgb="FFDDEBF7"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -209,15 +225,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF9BC2E6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF9BC2E6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -327,8 +356,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AD2" totalsRowShown="0">
-  <autoFilter ref="A1:AD2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AD22" totalsRowShown="0">
+  <autoFilter ref="A1:AD22" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="29"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Begintijd" dataDxfId="28"/>
@@ -339,27 +368,27 @@
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Welke opleiding volg je?" dataDxfId="23"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="In welk leerjaar zit je momenteel?" dataDxfId="22"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Heb je al een thuis-tentamen gemaakt?" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Hoe tevreden ben je met digitale tentamens als toetsvorm?" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Hoe tevreden ben je met papieren tentamens als toetsvorm?" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Wat is het grootste voordeel van een digitaal tentamen als toetsvorm?" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Wat is het grootste nadeel van een digitaal tentamen als toetsvorm?" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Ik kan me op een thuis tentamen net zo goed voorbereiden als een tentamen op de Hanze" dataDxfId="16"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Ik weet wat ik kan verwachten van een thuis tentamen" dataDxfId="15"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Welke hulpmiddelen ter voorbereiding zouden voor jou het meest behulpzaam zijn?" dataDxfId="14"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="De begeleiding van de surveillanten tijdens het thuis tentamen is goed" dataDxfId="13"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="De begeleiding vanuit mijn opleiding voor een thuis tentamen is goed " dataDxfId="12"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Ik kan me goed concentreren tijdens een thuis tentamen" dataDxfId="11"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="De thuis tentamens zijn goed georganiseerd" dataDxfId="10"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Ik kan goed mijn weg vinden (navigeren) in een digitaal tentamen" dataDxfId="9"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="De opstelling voor de livestream was makkelijk te maken" dataDxfId="8"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Ik vind het werken met de livestream gemakkelijk" dataDxfId="7"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Ik vind het prettig dat er een testsessie was" dataDxfId="6"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Heb je wel eens problemen gehad tijdens een thuis-tentamen?" dataDxfId="5"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Wat was er aan de hand, en hoe is dit toen opgelost?" dataDxfId="4"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Ik vind het belangrijk dat ik vanuit huis mijn tentamen kan inzien." dataDxfId="3"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Ik vind het belangrijk dat digitale tentamens worden nabesproken door de docent" dataDxfId="2"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Heb je nog opmerkingen of suggesties ten aanzien van thuis tentamens?" dataDxfId="1"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Wat vond je van deze vragenlijst?" dataDxfId="0"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Hoe tevreden ben je met digitale tentamens als toetsvorm?" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Hoe tevreden ben je met papieren tentamens als toetsvorm?" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Wat is het grootste voordeel van een digitaal tentamen als toetsvorm?" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Wat is het grootste nadeel van een digitaal tentamen als toetsvorm?" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Ik kan me op een thuis tentamen net zo goed voorbereiden als een tentamen op de Hanze" dataDxfId="17"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Ik weet wat ik kan verwachten van een thuis tentamen" dataDxfId="16"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Welke hulpmiddelen ter voorbereiding zouden voor jou het meest behulpzaam zijn?" dataDxfId="15"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="De begeleiding van de surveillanten tijdens het thuis tentamen is goed" dataDxfId="14"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="De begeleiding vanuit mijn opleiding voor een thuis tentamen is goed " dataDxfId="13"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Ik kan me goed concentreren tijdens een thuis tentamen" dataDxfId="12"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="De thuis tentamens zijn goed georganiseerd" dataDxfId="11"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Ik kan goed mijn weg vinden (navigeren) in een digitaal tentamen" dataDxfId="10"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="De opstelling voor de livestream was makkelijk te maken" dataDxfId="9"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Ik vind het werken met de livestream gemakkelijk" dataDxfId="8"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Ik vind het prettig dat er een testsessie was" dataDxfId="7"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Heb je wel eens problemen gehad tijdens een thuis-tentamen?" dataDxfId="6"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Wat was er aan de hand, en hoe is dit toen opgelost?" dataDxfId="5"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Ik vind het belangrijk dat ik vanuit huis mijn tentamen kan inzien." dataDxfId="4"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Ik vind het belangrijk dat digitale tentamens worden nabesproken door de docent" dataDxfId="3"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Heb je nog opmerkingen of suggesties ten aanzien van thuis tentamens?" dataDxfId="2"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Wat vond je van deze vragenlijst?" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -662,18 +691,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD3"/>
+  <dimension ref="A1:AD27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="AG22" sqref="AG22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="30" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -765,180 +794,1599 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43977.583518518499</v>
-      </c>
-      <c r="C2" s="1">
-        <v>43977.588668981502</v>
-      </c>
-      <c r="D2" s="3" t="s">
+    <row r="2" spans="1:30">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="J2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="K2">
-        <v>6</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>36</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
       <c r="N2" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>39</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="P2" s="3"/>
       <c r="Q2" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>41</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="Z2" s="3"/>
       <c r="AA2" s="3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>42</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="AC2" s="3"/>
       <c r="AD2">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A3">
+    <row r="3" spans="1:30">
+      <c r="A3" s="3"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3">
+        <v>6</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4">
+        <v>9</v>
+      </c>
+      <c r="K4">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>43977.633831018502</v>
-      </c>
-      <c r="C3" s="2">
-        <v>43977.6342939815</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="R4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z4" s="3"/>
+      <c r="AA4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+    </row>
+    <row r="5" spans="1:30">
+      <c r="A5" s="3"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+    </row>
+    <row r="6" spans="1:30">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+    </row>
+    <row r="7" spans="1:30">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J7">
+        <v>7</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+    </row>
+    <row r="8" spans="1:30">
+      <c r="A8" s="3"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="W8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="X8" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+    </row>
+    <row r="9" spans="1:30">
+      <c r="A9" s="3"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>3</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="S9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="X9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+    </row>
+    <row r="10" spans="1:30">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J10">
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V10" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="W10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+    </row>
+    <row r="11" spans="1:30">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J11">
+        <v>5</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X11" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+    </row>
+    <row r="12" spans="1:30">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12">
+        <v>5</v>
+      </c>
+      <c r="K12">
+        <v>10</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="S12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="W12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z12" s="3"/>
+      <c r="AA12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB12" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+    </row>
+    <row r="13" spans="1:30">
+      <c r="A13" s="3"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13">
+        <v>8</v>
+      </c>
+      <c r="K13">
+        <v>9</v>
+      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="V13" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="W13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X13" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z13" s="3"/>
+      <c r="AA13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+    </row>
+    <row r="14" spans="1:30">
+      <c r="A14" s="3"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>10</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="S14" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+    </row>
+    <row r="15" spans="1:30">
+      <c r="A15" s="3"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J15">
+        <v>5</v>
+      </c>
+      <c r="K15">
+        <v>7</v>
+      </c>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="W15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y15" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB15" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+    </row>
+    <row r="16" spans="1:30">
+      <c r="A16" s="3"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I3" t="s">
-        <v>34</v>
-      </c>
-      <c r="J3">
+      <c r="H16" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <v>6</v>
+      </c>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="S16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="T16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="U16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X16" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+    </row>
+    <row r="17" spans="1:30">
+      <c r="A17" s="3"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17">
+        <v>9</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="T17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="W17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y17" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+    </row>
+    <row r="18" spans="1:30">
+      <c r="A18" s="3"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J18">
+        <v>6</v>
+      </c>
+      <c r="K18">
         <v>5</v>
       </c>
-      <c r="K3">
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="S18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="T18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+    </row>
+    <row r="19" spans="1:30">
+      <c r="A19" s="3"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19">
+        <v>10</v>
+      </c>
+      <c r="K19">
+        <v>7</v>
+      </c>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="S19" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="T19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="U19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="W19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="X19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AB19" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+    </row>
+    <row r="20" spans="1:30">
+      <c r="A20" s="3"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J20">
+        <v>8</v>
+      </c>
+      <c r="K20">
+        <v>5</v>
+      </c>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="U20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="V20" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="W20" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z20" s="3"/>
+      <c r="AA20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+    </row>
+    <row r="21" spans="1:30">
+      <c r="A21" s="3"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21">
         <v>4</v>
       </c>
-      <c r="L3" t="s">
-        <v>45</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="K21">
+        <v>4</v>
+      </c>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="R21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S21" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="T21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="V21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="W21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="X21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z21" s="3"/>
+      <c r="AA21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+    </row>
+    <row r="22" spans="1:30">
+      <c r="A22" s="3"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="N3" t="s">
-        <v>47</v>
-      </c>
-      <c r="O3" t="s">
-        <v>47</v>
-      </c>
-      <c r="P3" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R3" t="s">
-        <v>47</v>
-      </c>
-      <c r="S3" t="s">
-        <v>47</v>
-      </c>
-      <c r="T3" t="s">
-        <v>47</v>
-      </c>
-      <c r="U3" t="s">
-        <v>47</v>
-      </c>
-      <c r="V3" t="s">
-        <v>47</v>
-      </c>
-      <c r="W3" t="s">
-        <v>47</v>
-      </c>
-      <c r="X3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD3">
+      <c r="H22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J22">
         <v>3</v>
       </c>
+      <c r="K22">
+        <v>6</v>
+      </c>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="T22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U22" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="V22" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z22" s="3"/>
+      <c r="AA22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+    </row>
+    <row r="23" spans="1:30">
+      <c r="A23" s="3"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+      <c r="V23" s="3"/>
+      <c r="W23" s="3"/>
+      <c r="X23" s="3"/>
+      <c r="Y23" s="3"/>
+      <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3"/>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+    </row>
+    <row r="24" spans="1:30">
+      <c r="A24" s="3"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
+      <c r="V24" s="3"/>
+      <c r="W24" s="3"/>
+      <c r="X24" s="3"/>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3"/>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+    </row>
+    <row r="25" spans="1:30">
+      <c r="A25" s="3"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="3"/>
+      <c r="U25" s="3"/>
+      <c r="V25" s="3"/>
+      <c r="W25" s="3"/>
+      <c r="X25" s="3"/>
+      <c r="Y25" s="3"/>
+      <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
+      <c r="AB25" s="3"/>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+    </row>
+    <row r="26" spans="1:30">
+      <c r="A26" s="3"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="3"/>
+      <c r="U26" s="3"/>
+      <c r="V26" s="3"/>
+      <c r="W26" s="3"/>
+      <c r="X26" s="3"/>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3"/>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+    </row>
+    <row r="27" spans="1:30">
+      <c r="A27" s="3"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="3"/>
+      <c r="U27" s="3"/>
+      <c r="V27" s="3"/>
+      <c r="W27" s="3"/>
+      <c r="X27" s="3"/>
+      <c r="Y27" s="3"/>
+      <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
+      <c r="AB27" s="3"/>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>